<commit_message>
added wisconsin data and figure
</commit_message>
<xml_diff>
--- a/florida_extended.xlsx
+++ b/florida_extended.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>Alachua</t>
   </si>
@@ -251,9 +251,6 @@
     <t>VTI as % of 2016 Total</t>
   </si>
   <si>
-    <t>Voter Turnout Increase (VTI)</t>
-  </si>
-  <si>
     <t>Digital Voting? (DVC)</t>
   </si>
   <si>
@@ -266,7 +263,7 @@
     <t>Democrat Voter Increase</t>
   </si>
   <si>
-    <t>Gained Significant Republican Votes?</t>
+    <t>Voter Turnout Change (VTI)</t>
   </si>
 </sst>
 </file>
@@ -843,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -889,23 +886,21 @@
         <v>70</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>74</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L1" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>80</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -941,8 +936,8 @@
         <v>7.7920888081295478E-2</v>
       </c>
       <c r="K2" s="29">
-        <f>$B2-$E2</f>
-        <v>-7578.6100000000006</v>
+        <f>$E2-$B2</f>
+        <v>7578.6100000000006</v>
       </c>
       <c r="L2" s="29">
         <f>$F2-$C2</f>
@@ -985,8 +980,8 @@
         <v>0.10785619174434088</v>
       </c>
       <c r="K3" s="29">
-        <f t="shared" ref="K3:K66" si="2">$B3-$E3</f>
-        <v>178.91100000000006</v>
+        <f t="shared" ref="K3:K66" si="2">$E3-$B3</f>
+        <v>-178.91100000000006</v>
       </c>
       <c r="L3" s="29">
         <f t="shared" ref="L3:L66" si="3">$F3-$C3</f>
@@ -1030,7 +1025,7 @@
       </c>
       <c r="K4" s="29">
         <f t="shared" si="2"/>
-        <v>-37.292000000001281</v>
+        <v>37.292000000001281</v>
       </c>
       <c r="L4" s="29">
         <f t="shared" si="3"/>
@@ -1074,7 +1069,7 @@
       </c>
       <c r="K5" s="29">
         <f t="shared" si="2"/>
-        <v>365.09799999999996</v>
+        <v>-365.09799999999996</v>
       </c>
       <c r="L5" s="29">
         <f t="shared" si="3"/>
@@ -1118,7 +1113,7 @@
       </c>
       <c r="K6" s="29">
         <f t="shared" si="2"/>
-        <v>1154.7400000000052</v>
+        <v>-1154.7400000000052</v>
       </c>
       <c r="L6" s="29">
         <f t="shared" si="3"/>
@@ -1162,7 +1157,7 @@
       </c>
       <c r="K7" s="29">
         <f t="shared" si="2"/>
-        <v>-52793.055000000051</v>
+        <v>52793.055000000051</v>
       </c>
       <c r="L7" s="29">
         <f t="shared" si="3"/>
@@ -1206,7 +1201,7 @@
       </c>
       <c r="K8" s="29">
         <f t="shared" si="2"/>
-        <v>399.81200000000013</v>
+        <v>-399.81200000000013</v>
       </c>
       <c r="L8" s="29">
         <f t="shared" si="3"/>
@@ -1250,7 +1245,7 @@
       </c>
       <c r="K9" s="29">
         <f t="shared" si="2"/>
-        <v>1839.9690000000046</v>
+        <v>-1839.9690000000046</v>
       </c>
       <c r="L9" s="29">
         <f t="shared" si="3"/>
@@ -1294,7 +1289,7 @@
       </c>
       <c r="K10" s="29">
         <f t="shared" si="2"/>
-        <v>5301.7220000000016</v>
+        <v>-5301.7220000000016</v>
       </c>
       <c r="L10" s="29">
         <f t="shared" si="3"/>
@@ -1338,7 +1333,7 @@
       </c>
       <c r="K11" s="29">
         <f t="shared" si="2"/>
-        <v>-2386.7180000000008</v>
+        <v>2386.7180000000008</v>
       </c>
       <c r="L11" s="29">
         <f t="shared" si="3"/>
@@ -1382,7 +1377,7 @@
       </c>
       <c r="K12" s="29">
         <f t="shared" si="2"/>
-        <v>-10598.5</v>
+        <v>10598.5</v>
       </c>
       <c r="L12" s="29">
         <f t="shared" si="3"/>
@@ -1426,7 +1421,7 @@
       </c>
       <c r="K13" s="29">
         <f t="shared" si="2"/>
-        <v>772.75999999999931</v>
+        <v>-772.75999999999931</v>
       </c>
       <c r="L13" s="29">
         <f t="shared" si="3"/>
@@ -1470,7 +1465,7 @@
       </c>
       <c r="K14" s="29">
         <f t="shared" si="2"/>
-        <v>337.44300000000021</v>
+        <v>-337.44300000000021</v>
       </c>
       <c r="L14" s="29">
         <f t="shared" si="3"/>
@@ -1514,7 +1509,7 @@
       </c>
       <c r="K15" s="29">
         <f t="shared" si="2"/>
-        <v>516.36800000000017</v>
+        <v>-516.36800000000017</v>
       </c>
       <c r="L15" s="29">
         <f t="shared" si="3"/>
@@ -1558,7 +1553,7 @@
       </c>
       <c r="K16" s="29">
         <f t="shared" si="2"/>
-        <v>-11760.449999999983</v>
+        <v>11760.449999999983</v>
       </c>
       <c r="L16" s="29">
         <f t="shared" si="3"/>
@@ -1602,7 +1597,7 @@
       </c>
       <c r="K17" s="29">
         <f t="shared" si="2"/>
-        <v>-332.18600000000151</v>
+        <v>332.18600000000151</v>
       </c>
       <c r="L17" s="29">
         <f t="shared" si="3"/>
@@ -1646,7 +1641,7 @@
       </c>
       <c r="K18" s="29">
         <f t="shared" si="2"/>
-        <v>839.03399999999965</v>
+        <v>-839.03399999999965</v>
       </c>
       <c r="L18" s="29">
         <f t="shared" si="3"/>
@@ -1690,7 +1685,7 @@
       </c>
       <c r="K19" s="29">
         <f t="shared" si="2"/>
-        <v>73.680000000000064</v>
+        <v>-73.680000000000064</v>
       </c>
       <c r="L19" s="29">
         <f t="shared" si="3"/>
@@ -1734,7 +1729,7 @@
       </c>
       <c r="K20" s="29">
         <f t="shared" si="2"/>
-        <v>604.53499999999804</v>
+        <v>-604.53499999999804</v>
       </c>
       <c r="L20" s="29">
         <f t="shared" si="3"/>
@@ -1778,7 +1773,7 @@
       </c>
       <c r="K21" s="29">
         <f t="shared" si="2"/>
-        <v>411.7320000000002</v>
+        <v>-411.7320000000002</v>
       </c>
       <c r="L21" s="29">
         <f t="shared" si="3"/>
@@ -1822,7 +1817,7 @@
       </c>
       <c r="K22" s="29">
         <f t="shared" si="2"/>
-        <v>314.11200000000008</v>
+        <v>-314.11200000000008</v>
       </c>
       <c r="L22" s="29">
         <f t="shared" si="3"/>
@@ -1866,7 +1861,7 @@
       </c>
       <c r="K23" s="29">
         <f t="shared" si="2"/>
-        <v>273.5</v>
+        <v>-273.5</v>
       </c>
       <c r="L23" s="29">
         <f t="shared" si="3"/>
@@ -1910,7 +1905,7 @@
       </c>
       <c r="K24" s="29">
         <f t="shared" si="2"/>
-        <v>303.56000000000017</v>
+        <v>-303.56000000000017</v>
       </c>
       <c r="L24" s="29">
         <f t="shared" si="3"/>
@@ -1954,7 +1949,7 @@
       </c>
       <c r="K25" s="29">
         <f t="shared" si="2"/>
-        <v>283.90000000000009</v>
+        <v>-283.90000000000009</v>
       </c>
       <c r="L25" s="29">
         <f t="shared" si="3"/>
@@ -1998,7 +1993,7 @@
       </c>
       <c r="K26" s="29">
         <f t="shared" si="2"/>
-        <v>75.610000000000582</v>
+        <v>-75.610000000000582</v>
       </c>
       <c r="L26" s="29">
         <f t="shared" si="3"/>
@@ -2042,7 +2037,7 @@
       </c>
       <c r="K27" s="29">
         <f t="shared" si="2"/>
-        <v>5515.163999999997</v>
+        <v>-5515.163999999997</v>
       </c>
       <c r="L27" s="29">
         <f t="shared" si="3"/>
@@ -2086,7 +2081,7 @@
       </c>
       <c r="K28" s="29">
         <f t="shared" si="2"/>
-        <v>981.08599999999933</v>
+        <v>-981.08599999999933</v>
       </c>
       <c r="L28" s="29">
         <f t="shared" si="3"/>
@@ -2130,7 +2125,7 @@
       </c>
       <c r="K29" s="29">
         <f t="shared" si="2"/>
-        <v>-26788.445000000007</v>
+        <v>26788.445000000007</v>
       </c>
       <c r="L29" s="29">
         <f t="shared" si="3"/>
@@ -2174,7 +2169,7 @@
       </c>
       <c r="K30" s="29">
         <f t="shared" si="2"/>
-        <v>401.79999999999995</v>
+        <v>-401.79999999999995</v>
       </c>
       <c r="L30" s="29">
         <f t="shared" si="3"/>
@@ -2218,7 +2213,7 @@
       </c>
       <c r="K31" s="29">
         <f t="shared" si="2"/>
-        <v>-2170.9079999999994</v>
+        <v>2170.9079999999994</v>
       </c>
       <c r="L31" s="29">
         <f t="shared" si="3"/>
@@ -2262,7 +2257,7 @@
       </c>
       <c r="K32" s="29">
         <f t="shared" si="2"/>
-        <v>870.75200000000041</v>
+        <v>-870.75200000000041</v>
       </c>
       <c r="L32" s="29">
         <f t="shared" si="3"/>
@@ -2306,7 +2301,7 @@
       </c>
       <c r="K33" s="29">
         <f t="shared" si="2"/>
-        <v>355.36099999999988</v>
+        <v>-355.36099999999988</v>
       </c>
       <c r="L33" s="29">
         <f t="shared" si="3"/>
@@ -2350,7 +2345,7 @@
       </c>
       <c r="K34" s="29">
         <f t="shared" si="2"/>
-        <v>160.83299999999997</v>
+        <v>-160.83299999999997</v>
       </c>
       <c r="L34" s="29">
         <f t="shared" si="3"/>
@@ -2394,7 +2389,7 @@
       </c>
       <c r="K35" s="29">
         <f t="shared" si="2"/>
-        <v>-1950.0080000000016</v>
+        <v>1950.0080000000016</v>
       </c>
       <c r="L35" s="29">
         <f t="shared" si="3"/>
@@ -2438,7 +2433,7 @@
       </c>
       <c r="K36" s="29">
         <f t="shared" si="2"/>
-        <v>-17319.188000000009</v>
+        <v>17319.188000000009</v>
       </c>
       <c r="L36" s="29">
         <f t="shared" si="3"/>
@@ -2482,7 +2477,7 @@
       </c>
       <c r="K37" s="29">
         <f t="shared" si="2"/>
-        <v>-2927.2749999999942</v>
+        <v>2927.2749999999942</v>
       </c>
       <c r="L37" s="29">
         <f t="shared" si="3"/>
@@ -2526,7 +2521,7 @@
       </c>
       <c r="K38" s="29">
         <f t="shared" si="2"/>
-        <v>963.41100000000006</v>
+        <v>-963.41100000000006</v>
       </c>
       <c r="L38" s="29">
         <f t="shared" si="3"/>
@@ -2570,7 +2565,7 @@
       </c>
       <c r="K39" s="29">
         <f t="shared" si="2"/>
-        <v>278.89800000000002</v>
+        <v>-278.89800000000002</v>
       </c>
       <c r="L39" s="29">
         <f t="shared" si="3"/>
@@ -2614,7 +2609,7 @@
       </c>
       <c r="K40" s="29">
         <f t="shared" si="2"/>
-        <v>606.58500000000004</v>
+        <v>-606.58500000000004</v>
       </c>
       <c r="L40" s="29">
         <f t="shared" si="3"/>
@@ -2658,7 +2653,7 @@
       </c>
       <c r="K41" s="29">
         <f t="shared" si="2"/>
-        <v>-6003.8439999999973</v>
+        <v>6003.8439999999973</v>
       </c>
       <c r="L41" s="29">
         <f t="shared" si="3"/>
@@ -2702,7 +2697,7 @@
       </c>
       <c r="K42" s="29">
         <f t="shared" si="2"/>
-        <v>3936.3600000000006</v>
+        <v>-3936.3600000000006</v>
       </c>
       <c r="L42" s="29">
         <f t="shared" si="3"/>
@@ -2746,7 +2741,7 @@
       </c>
       <c r="K43" s="29">
         <f t="shared" si="2"/>
-        <v>-705.31999999999971</v>
+        <v>705.31999999999971</v>
       </c>
       <c r="L43" s="29">
         <f t="shared" si="3"/>
@@ -2790,7 +2785,7 @@
       </c>
       <c r="K44" s="29">
         <f t="shared" si="2"/>
-        <v>-94671.385000000009</v>
+        <v>94671.385000000009</v>
       </c>
       <c r="L44" s="29">
         <f t="shared" si="3"/>
@@ -2834,7 +2829,7 @@
       </c>
       <c r="K45" s="29">
         <f t="shared" si="2"/>
-        <v>24.31499999999869</v>
+        <v>-24.31499999999869</v>
       </c>
       <c r="L45" s="29">
         <f t="shared" si="3"/>
@@ -2878,7 +2873,7 @@
       </c>
       <c r="K46" s="29">
         <f t="shared" si="2"/>
-        <v>-761.04600000000028</v>
+        <v>761.04600000000028</v>
       </c>
       <c r="L46" s="29">
         <f t="shared" si="3"/>
@@ -2922,7 +2917,7 @@
       </c>
       <c r="K47" s="29">
         <f t="shared" si="2"/>
-        <v>-810.29999999999927</v>
+        <v>810.29999999999927</v>
       </c>
       <c r="L47" s="29">
         <f t="shared" si="3"/>
@@ -2966,7 +2961,7 @@
       </c>
       <c r="K48" s="29">
         <f t="shared" si="2"/>
-        <v>836.89000000000033</v>
+        <v>-836.89000000000033</v>
       </c>
       <c r="L48" s="29">
         <f t="shared" si="3"/>
@@ -3010,7 +3005,7 @@
       </c>
       <c r="K49" s="29">
         <f t="shared" si="2"/>
-        <v>-62239.935999999987</v>
+        <v>62239.935999999987</v>
       </c>
       <c r="L49" s="29">
         <f t="shared" si="3"/>
@@ -3054,7 +3049,7 @@
       </c>
       <c r="K50" s="29">
         <f t="shared" si="2"/>
-        <v>-19665.300000000003</v>
+        <v>19665.300000000003</v>
       </c>
       <c r="L50" s="29">
         <f t="shared" si="3"/>
@@ -3098,7 +3093,7 @@
       </c>
       <c r="K51" s="29">
         <f t="shared" si="2"/>
-        <v>-30371.954999999958</v>
+        <v>30371.954999999958</v>
       </c>
       <c r="L51" s="29">
         <f t="shared" si="3"/>
@@ -3142,7 +3137,7 @@
       </c>
       <c r="K52" s="29">
         <f t="shared" si="2"/>
-        <v>6651.6999999999971</v>
+        <v>-6651.6999999999971</v>
       </c>
       <c r="L52" s="29">
         <f t="shared" si="3"/>
@@ -3186,7 +3181,7 @@
       </c>
       <c r="K53" s="29">
         <f t="shared" si="2"/>
-        <v>600.32500000001164</v>
+        <v>-600.32500000001164</v>
       </c>
       <c r="L53" s="29">
         <f t="shared" si="3"/>
@@ -3230,7 +3225,7 @@
       </c>
       <c r="K54" s="29">
         <f t="shared" si="2"/>
-        <v>-4763.083999999988</v>
+        <v>4763.083999999988</v>
       </c>
       <c r="L54" s="29">
         <f t="shared" si="3"/>
@@ -3274,7 +3269,7 @@
       </c>
       <c r="K55" s="29">
         <f t="shared" si="2"/>
-        <v>1486.648000000001</v>
+        <v>-1486.648000000001</v>
       </c>
       <c r="L55" s="29">
         <f t="shared" si="3"/>
@@ -3318,7 +3313,7 @@
       </c>
       <c r="K56" s="29">
         <f t="shared" si="2"/>
-        <v>-943.84000000000015</v>
+        <v>943.84000000000015</v>
       </c>
       <c r="L56" s="29">
         <f t="shared" si="3"/>
@@ -3362,7 +3357,7 @@
       </c>
       <c r="K57" s="29">
         <f t="shared" si="2"/>
-        <v>-4559.025999999998</v>
+        <v>4559.025999999998</v>
       </c>
       <c r="L57" s="29">
         <f t="shared" si="3"/>
@@ -3406,7 +3401,7 @@
       </c>
       <c r="K58" s="29">
         <f t="shared" si="2"/>
-        <v>-11522.800999999992</v>
+        <v>11522.800999999992</v>
       </c>
       <c r="L58" s="29">
         <f t="shared" si="3"/>
@@ -3450,7 +3445,7 @@
       </c>
       <c r="K59" s="29">
         <f t="shared" si="2"/>
-        <v>-8627.8240000000005</v>
+        <v>8627.8240000000005</v>
       </c>
       <c r="L59" s="29">
         <f t="shared" si="3"/>
@@ -3494,7 +3489,7 @@
       </c>
       <c r="K60" s="29">
         <f t="shared" si="2"/>
-        <v>-2083.0749999999971</v>
+        <v>2083.0749999999971</v>
       </c>
       <c r="L60" s="29">
         <f t="shared" si="3"/>
@@ -3538,7 +3533,7 @@
       </c>
       <c r="K61" s="29">
         <f t="shared" si="2"/>
-        <v>-3430.244999999999</v>
+        <v>3430.244999999999</v>
       </c>
       <c r="L61" s="29">
         <f t="shared" si="3"/>
@@ -3582,7 +3577,7 @@
       </c>
       <c r="K62" s="29">
         <f t="shared" si="2"/>
-        <v>743.35200000000032</v>
+        <v>-743.35200000000032</v>
       </c>
       <c r="L62" s="29">
         <f t="shared" si="3"/>
@@ -3626,7 +3621,7 @@
       </c>
       <c r="K63" s="29">
         <f t="shared" si="2"/>
-        <v>581.34400000000005</v>
+        <v>-581.34400000000005</v>
       </c>
       <c r="L63" s="29">
         <f t="shared" si="3"/>
@@ -3670,7 +3665,7 @@
       </c>
       <c r="K64" s="29">
         <f t="shared" si="2"/>
-        <v>314.61000000000013</v>
+        <v>-314.61000000000013</v>
       </c>
       <c r="L64" s="29">
         <f t="shared" si="3"/>
@@ -3714,7 +3709,7 @@
       </c>
       <c r="K65" s="29">
         <f t="shared" si="2"/>
-        <v>3893.5639999999985</v>
+        <v>-3893.5639999999985</v>
       </c>
       <c r="L65" s="29">
         <f t="shared" si="3"/>
@@ -3758,7 +3753,7 @@
       </c>
       <c r="K66" s="29">
         <f t="shared" si="2"/>
-        <v>780.85900000000038</v>
+        <v>-780.85900000000038</v>
       </c>
       <c r="L66" s="29">
         <f t="shared" si="3"/>
@@ -3801,8 +3796,8 @@
         <v>0.1613262910798122</v>
       </c>
       <c r="K67" s="29">
-        <f t="shared" ref="K67:K68" si="6">$B67-$E67</f>
-        <v>-281.31999999999971</v>
+        <f t="shared" ref="K67:K68" si="6">$E67-$B67</f>
+        <v>281.31999999999971</v>
       </c>
       <c r="L67" s="29">
         <f t="shared" ref="L67:L68" si="7">$F67-$C67</f>
@@ -3846,7 +3841,7 @@
       </c>
       <c r="K68" s="29">
         <f t="shared" si="6"/>
-        <v>527.52099999999973</v>
+        <v>-527.52099999999973</v>
       </c>
       <c r="L68" s="29">
         <f t="shared" si="7"/>
@@ -3881,14 +3876,14 @@
     </row>
     <row r="70" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C70" s="1">
         <f>MAX(B69,C69)/(SUM(B69,C69))</f>
         <v>0.50442252139366228</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F70" s="1">
         <f>MAX(E69,F69)/(SUM(E69,F69))</f>

</xml_diff>